<commit_message>
update main.py and app.py
</commit_message>
<xml_diff>
--- a/data/recommendartion_data/finalIndonesia_data2.xlsx
+++ b/data/recommendartion_data/finalIndonesia_data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODING\Project Capstone Bisa AI\data\recommendartion_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A932A0EF-4471-4962-BD5A-A7037297EF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E1BB11-B6D8-45C4-81B6-3E00F43627F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,9 +844,6 @@
     <t>https://tse3.mm.bing.net/th/id/OIP.gKA50I6rJgN3YdGZ9ctygwHaHa?pid=ImgDet</t>
   </si>
   <si>
-    <t>-, 2428.7856, 600.0, -</t>
-  </si>
-  <si>
     <t>Daging Sapi Pedas dalam Kelapa (Rendang Daging Sapi)</t>
   </si>
   <si>
@@ -887,6 +884,9 @@
   </si>
   <si>
     <t>Kue Cokelat Chip "Indonesia".</t>
+  </si>
+  <si>
+    <t>1100.0, 2428.7856, 600.0, 600.0</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1614,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C26" t="s">
         <v>74</v>
@@ -2426,7 +2426,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C84" t="s">
         <v>238</v>
@@ -2538,7 +2538,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C92" t="s">
         <v>261</v>
@@ -2600,7 +2600,7 @@
         <v>273</v>
       </c>
       <c r="D96" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2608,13 +2608,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C97" t="s">
         <v>158</v>
       </c>
       <c r="D97" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2622,13 +2622,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
+        <v>276</v>
+      </c>
+      <c r="C98" t="s">
         <v>277</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>278</v>
-      </c>
-      <c r="D98" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2636,10 +2636,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
+        <v>279</v>
+      </c>
+      <c r="C99" t="s">
         <v>280</v>
-      </c>
-      <c r="C99" t="s">
-        <v>281</v>
       </c>
       <c r="D99" t="s">
         <v>156</v>
@@ -2650,10 +2650,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
+        <v>281</v>
+      </c>
+      <c r="C100" t="s">
         <v>282</v>
-      </c>
-      <c r="C100" t="s">
-        <v>283</v>
       </c>
       <c r="D100" t="s">
         <v>156</v>
@@ -2664,10 +2664,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
+        <v>283</v>
+      </c>
+      <c r="C101" t="s">
         <v>284</v>
-      </c>
-      <c r="C101" t="s">
-        <v>285</v>
       </c>
       <c r="D101" t="s">
         <v>156</v>

</xml_diff>